<commit_message>
Integração com o banco de dados
</commit_message>
<xml_diff>
--- a/Config_Grade.xlsx
+++ b/Config_Grade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\Workspaces\Secretaria-Workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaeldbo1\Downloads\code\grade_graduacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009CB4DE-9173-482D-AC49-56DC8B974B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD3E4C5-2D04-4069-894A-AE59ACA8EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -33,8 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="112">
   <si>
     <t>Tipo</t>
   </si>
@@ -125,24 +123,6 @@
     <t>Cursos</t>
   </si>
   <si>
-    <t>GRADM</t>
-  </si>
-  <si>
-    <t>GRECO</t>
-  </si>
-  <si>
-    <t>GRENGCOMP</t>
-  </si>
-  <si>
-    <t>GRENGMECAT</t>
-  </si>
-  <si>
-    <t>GRDIR</t>
-  </si>
-  <si>
-    <t>GRCIECOMP</t>
-  </si>
-  <si>
     <t>Tipos de Aula</t>
   </si>
   <si>
@@ -251,9 +231,6 @@
     <t/>
   </si>
   <si>
-    <t>CAPSTONE</t>
-  </si>
-  <si>
     <t>Agendado como Capstone de Eng. Comp.</t>
   </si>
   <si>
@@ -279,9 +256,6 @@
   </si>
   <si>
     <t>Diferenciação de Curso</t>
-  </si>
-  <si>
-    <t>GRENGMECA</t>
   </si>
   <si>
     <t>Dia Reservado</t>
@@ -376,13 +350,43 @@
   </si>
   <si>
     <t>MICROECONOMIA I</t>
+  </si>
+  <si>
+    <t>CIECOMP</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>MECAT</t>
+  </si>
+  <si>
+    <t>MECA</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>ECO</t>
+  </si>
+  <si>
+    <t>ADM</t>
+  </si>
+  <si>
+    <t>ADM/ECO</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>MECA/MECAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +437,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -460,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,9 +500,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -500,6 +508,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,21 +857,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ACDB79-7005-4B8E-AC77-4D96767B7990}">
-  <dimension ref="AA1:AD10"/>
+  <dimension ref="AA1:AD11"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="27" max="27" width="37.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="37.9140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.9140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.9140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="27:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="27:30">
       <c r="AA1" s="8" t="s">
         <v>25</v>
       </c>
@@ -862,112 +879,120 @@
         <v>26</v>
       </c>
       <c r="AC1" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="AD1" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="27:30" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="27:30">
       <c r="AA2" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="27:30" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="27:30">
       <c r="AA3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="AB3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="AD3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="27:30" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="27:30">
       <c r="AA4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="27:30" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="27:30">
       <c r="AA5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="27:30">
+      <c r="AA6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="27:30">
+      <c r="AA7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AB5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA7" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC7" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="27:30" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="27:30">
       <c r="AA8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="27:30">
+      <c r="AA9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AB8" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA9" s="4" t="s">
+      <c r="AB9" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="27:30">
+      <c r="AA10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="27:30">
+      <c r="AB11" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="27:30" x14ac:dyDescent="0.3">
-      <c r="AA10" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -979,331 +1004,330 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="37.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.77734375" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="37.9140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.58203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.75" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.9140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="28">
       <c r="B1" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="28">
+      <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="11" t="s">
+      <c r="B24" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="11" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="28">
+      <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>38</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:C2" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1323,40 +1347,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8DDCAC-6EF5-4B90-A60D-BF7A19FDB345}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J29" sqref="A22:J29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.4140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
     <col min="9" max="9" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.6640625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="11" max="16384" width="8.9140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="28">
       <c r="D1" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1373,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>23</v>
@@ -1388,24 +1412,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="42">
       <c r="A3" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G3" s="7">
         <v>0.41666666666666669</v>
@@ -1413,31 +1437,31 @@
       <c r="H3" s="7">
         <v>0.5</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>68</v>
+      <c r="I3" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="42">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" s="7">
         <v>0.41666666666666669</v>
@@ -1446,27 +1470,27 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="42">
       <c r="A5" s="4" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G5" s="7">
         <v>0.41666666666666669</v>
@@ -1474,31 +1498,31 @@
       <c r="H5" s="7">
         <v>0.5</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>68</v>
+      <c r="I5" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="42">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G6" s="7">
         <v>0.41666666666666669</v>
@@ -1506,61 +1530,61 @@
       <c r="H6" s="7">
         <v>0.5</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>68</v>
+      <c r="I6" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="28">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G7" s="7">
         <v>0.3125</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="13">
         <v>0.75</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="28">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G8" s="7">
         <v>0.3125</v>
@@ -1569,27 +1593,27 @@
         <v>0.75</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="28">
       <c r="A9" s="4" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G9" s="7">
         <v>0.3125</v>
@@ -1598,27 +1622,27 @@
         <v>0.75</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="28">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G10" s="7">
         <v>0.3125</v>
@@ -1627,27 +1651,27 @@
         <v>0.75</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="28">
       <c r="A11" s="4" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B11" s="4">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G11" s="7">
         <v>0.64583333333333337</v>
@@ -1656,30 +1680,30 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="28">
       <c r="A12" s="4" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B12" s="4">
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G12" s="7">
         <v>0.40625</v>
@@ -1688,30 +1712,30 @@
         <v>0.46875</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="42">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B13" s="4">
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G13" s="7">
         <v>0.33333333333333331</v>
@@ -1720,30 +1744,30 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="28">
       <c r="A14" s="4" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B14" s="4">
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G14" s="7">
         <v>0.40625</v>
@@ -1752,30 +1776,30 @@
         <v>0.46875</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="28">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B15" s="4">
         <v>5</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G15" s="7">
         <v>0.41666666666666669</v>
@@ -1784,30 +1808,30 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="28">
       <c r="A16" s="4" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4">
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G16" s="7">
         <v>0.3125</v>
@@ -1816,30 +1840,30 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28">
       <c r="A17" s="4" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B17" s="4">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G17" s="7">
         <v>0.5625</v>
@@ -1848,30 +1872,30 @@
         <v>0.625</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B18" s="4">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G18" s="7">
         <v>0.64583333333333337</v>
@@ -1880,30 +1904,30 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="28">
       <c r="A19" s="4" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B19" s="4">
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G19" s="7">
         <v>0.33333333333333331</v>
@@ -1912,30 +1936,30 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B20" s="4">
         <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G20" s="7">
         <v>0.3125</v>
@@ -1944,27 +1968,27 @@
         <v>0.75</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="28">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="B21" s="4">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="G21" s="7">
         <v>0.3125</v>
@@ -1973,27 +1997,27 @@
         <v>0.75</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="28">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G22" s="7">
         <v>0.3125</v>
@@ -2002,30 +2026,30 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G23" s="7">
         <v>0.5625</v>
@@ -2034,30 +2058,30 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G24" s="7">
         <v>0.40625</v>
@@ -2066,30 +2090,30 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28">
       <c r="A25" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G25" s="7">
         <v>0.65625</v>
@@ -2098,30 +2122,30 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="28">
       <c r="A26" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G26" s="7">
         <v>0.5625</v>
@@ -2130,30 +2154,30 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28">
       <c r="A27" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G27" s="7">
         <v>0.40625</v>
@@ -2162,30 +2186,30 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28">
       <c r="A28" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G28" s="7">
         <v>0.65625</v>
@@ -2194,30 +2218,30 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="28">
       <c r="A29" s="4" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G29" s="7">
         <v>0.3125</v>
@@ -2226,25 +2250,20 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:J2" xr:uid="{1D8DDCAC-6EF5-4B90-A60D-BF7A19FDB345}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5137D3DF-26AE-4AF5-9132-45D721A70127}">
-          <x14:formula1>
-            <xm:f>Planilha2!$AB$2:$AB$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A1048576</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDF9556-88DF-433E-B10B-FEACDE6B4639}">
           <x14:formula1>
             <xm:f>Planilha2!$AC$2:$AC$7</xm:f>
@@ -2257,6 +2276,12 @@
           </x14:formula1>
           <xm:sqref>F3:F1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5137D3DF-26AE-4AF5-9132-45D721A70127}">
+          <x14:formula1>
+            <xm:f>Planilha2!$AB$2:$AB$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Adicionando remoção de aulas
</commit_message>
<xml_diff>
--- a/Config_Grade.xlsx
+++ b/Config_Grade.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaeldbo1\Downloads\code\grade_graduacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD3E4C5-2D04-4069-894A-AE59ACA8EF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B10FF1-140A-4F8B-8CC3-3ADA7AA58271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
     <sheet name="Dados Configuráveis" sheetId="1" r:id="rId2"/>
-    <sheet name="Horários Manuais" sheetId="3" r:id="rId3"/>
+    <sheet name="Adição Horários Manuais" sheetId="3" r:id="rId3"/>
+    <sheet name="Remoção Horários Space" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Adição Horários Manuais'!$A$2:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dados Configuráveis'!$A$2:$C$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Horários Manuais'!$A$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="100">
   <si>
     <t>Tipo</t>
   </si>
@@ -96,9 +97,6 @@
     <t>Disciplina com 2 Atendimentos</t>
   </si>
   <si>
-    <t>Disciplina</t>
-  </si>
-  <si>
     <t>Docente</t>
   </si>
   <si>
@@ -108,9 +106,6 @@
     <t>Série</t>
   </si>
   <si>
-    <t>Turma Pref</t>
-  </si>
-  <si>
     <t>Hora início</t>
   </si>
   <si>
@@ -144,9 +139,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>MODELAGEM E CONTROLE</t>
-  </si>
-  <si>
     <t>Formato HH:MM (Sem Tempo Pré)</t>
   </si>
   <si>
@@ -159,9 +151,6 @@
     <t>Nome do Docente que aparecerá na Grade</t>
   </si>
   <si>
-    <t>VINICIUS LICKS</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -184,45 +173,6 @@
   </si>
   <si>
     <t>Sexta-feira</t>
-  </si>
-  <si>
-    <t>CARLOS EDUARDO DE BRITO NOVAES</t>
-  </si>
-  <si>
-    <t>Sala do Professor</t>
-  </si>
-  <si>
-    <t>TRANSFERÊNCIA DE CALOR E MECÂNICA DOS SÓLIDOS</t>
-  </si>
-  <si>
-    <t>CAIO FERNANDO RODRIGUES DOS SANTOS</t>
-  </si>
-  <si>
-    <t>DESAFIOS DE PROGRAMAÇÃO</t>
-  </si>
-  <si>
-    <t>MARCELO HASHIMOTO</t>
-  </si>
-  <si>
-    <t>MÉTODOS NUMÉRICOS</t>
-  </si>
-  <si>
-    <t>PROJETO BIOMECÂNICO</t>
-  </si>
-  <si>
-    <t>FABIO TURRI</t>
-  </si>
-  <si>
-    <t>Agendamento não Recorrente no Space</t>
-  </si>
-  <si>
-    <t>TRANSFERÊNCIA DE CALOR</t>
-  </si>
-  <si>
-    <t>CONTROLE CLÁSSICO</t>
-  </si>
-  <si>
-    <t>CONTROLE MODERNO</t>
   </si>
   <si>
     <t>PROJETO FINAL - CAPSTONE</t>
@@ -380,6 +330,21 @@
   </si>
   <si>
     <t>MECA/MECAT</t>
+  </si>
+  <si>
+    <t>Turma</t>
+  </si>
+  <si>
+    <t>Código da Disciplina</t>
+  </si>
+  <si>
+    <t>Nome Disciplina</t>
+  </si>
+  <si>
+    <t>Tipo Atividade</t>
+  </si>
+  <si>
+    <t>GRENGCOM_201561_0023</t>
   </si>
 </sst>
 </file>
@@ -873,30 +838,30 @@
   <sheetData>
     <row r="1" spans="27:30">
       <c r="AA1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="AD1" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="27:30">
       <c r="AA2" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="27:30">
@@ -904,13 +869,13 @@
         <v>16</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="27:30">
@@ -918,81 +883,81 @@
         <v>17</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AD4" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="27:30">
       <c r="AA5" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="AD5" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="27:30">
       <c r="AA6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="27:30">
       <c r="AA7" s="4" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="27:30">
       <c r="AA8" s="4" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="27:30">
       <c r="AA9" s="4" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="27:30">
       <c r="AA10" s="4" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="27:30">
       <c r="AB11" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -1018,7 +983,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="28">
       <c r="B1" s="5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1">
@@ -1034,7 +999,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>5</v>
@@ -1042,7 +1007,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
@@ -1050,7 +1015,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>7</v>
@@ -1058,7 +1023,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>8</v>
@@ -1066,7 +1031,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>9</v>
@@ -1114,7 +1079,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>6</v>
@@ -1122,7 +1087,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>7</v>
@@ -1130,7 +1095,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>8</v>
@@ -1138,7 +1103,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>3</v>
@@ -1146,7 +1111,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>4</v>
@@ -1154,7 +1119,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
@@ -1162,66 +1127,66 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28">
       <c r="A24" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1229,95 +1194,95 @@
         <v>16</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28">
       <c r="A36" s="3" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1345,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8DDCAC-6EF5-4B90-A60D-BF7A19FDB345}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
@@ -1357,7 +1322,7 @@
     <col min="2" max="2" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.4140625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.4140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="18.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
@@ -1368,45 +1333,45 @@
   <sheetData>
     <row r="1" spans="1:15" s="5" customFormat="1" ht="28">
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>1</v>
@@ -1414,22 +1379,22 @@
     </row>
     <row r="3" spans="1:15" ht="42">
       <c r="A3" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G3" s="7">
         <v>0.41666666666666669</v>
@@ -1438,30 +1403,30 @@
         <v>0.5</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="42">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G4" s="7">
         <v>0.41666666666666669</v>
@@ -1470,27 +1435,27 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="42">
       <c r="A5" s="4" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G5" s="7">
         <v>0.41666666666666669</v>
@@ -1499,30 +1464,30 @@
         <v>0.5</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="42">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G6" s="7">
         <v>0.41666666666666669</v>
@@ -1531,30 +1496,30 @@
         <v>0.5</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="28">
       <c r="A7" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G7" s="7">
         <v>0.3125</v>
@@ -1563,28 +1528,28 @@
         <v>0.75</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" ht="28">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G8" s="7">
         <v>0.3125</v>
@@ -1593,27 +1558,27 @@
         <v>0.75</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="28">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G9" s="7">
         <v>0.3125</v>
@@ -1622,27 +1587,27 @@
         <v>0.75</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28">
       <c r="A10" s="4" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G10" s="7">
         <v>0.3125</v>
@@ -1651,609 +1616,321 @@
         <v>0.75</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="28">
       <c r="A11" s="4" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B11" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="7">
-        <v>0.64583333333333337</v>
+        <v>0.3125</v>
       </c>
       <c r="H11" s="7">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>39</v>
+        <v>0.75</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="28">
       <c r="A12" s="4" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B12" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.3125</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="28">
+      <c r="A13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.40625</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0.46875</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="42">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4">
-        <v>5</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G13" s="7">
-        <v>0.33333333333333331</v>
+        <v>0.3125</v>
       </c>
       <c r="H13" s="7">
         <v>0.39583333333333331</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="28">
       <c r="A14" s="4" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G14" s="7">
-        <v>0.40625</v>
+        <v>0.5625</v>
       </c>
       <c r="H14" s="7">
-        <v>0.46875</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="28">
       <c r="A15" s="4" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B15" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7">
-        <v>0.41666666666666669</v>
+        <v>0.40625</v>
       </c>
       <c r="H15" s="7">
-        <v>0.47916666666666669</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="28">
       <c r="A16" s="4" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B16" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G16" s="7">
-        <v>0.3125</v>
+        <v>0.65625</v>
       </c>
       <c r="H16" s="7">
-        <v>0.39583333333333331</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="28">
       <c r="A17" s="4" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B17" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G17" s="7">
         <v>0.5625</v>
       </c>
       <c r="H17" s="7">
-        <v>0.625</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28">
       <c r="A18" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B18" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G18" s="7">
-        <v>0.64583333333333337</v>
+        <v>0.40625</v>
       </c>
       <c r="H18" s="7">
-        <v>0.70833333333333337</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="28">
       <c r="A19" s="4" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G19" s="7">
-        <v>0.33333333333333331</v>
+        <v>0.65625</v>
       </c>
       <c r="H19" s="7">
-        <v>0.39583333333333331</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="28">
       <c r="A20" s="4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B20" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G20" s="7">
         <v>0.3125</v>
       </c>
       <c r="H20" s="7">
-        <v>0.75</v>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28">
-      <c r="A21" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B21" s="4">
-        <v>6</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="7">
-        <v>0.3125</v>
-      </c>
-      <c r="H21" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28">
-      <c r="A22" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G22" s="7">
-        <v>0.3125</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28">
-      <c r="A23" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="7">
-        <v>0.5625</v>
-      </c>
-      <c r="H23" s="7">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28">
-      <c r="A24" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="4">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0.40625</v>
-      </c>
-      <c r="H24" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="I24" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28">
-      <c r="A25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="7">
-        <v>0.65625</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28">
-      <c r="A26" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G26" s="7">
-        <v>0.5625</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28">
-      <c r="A27" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0.40625</v>
-      </c>
-      <c r="H27" s="7">
-        <v>0.48958333333333331</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28">
-      <c r="A28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0.65625</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28">
-      <c r="A29" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="7">
-        <v>0.3125</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2286,4 +1963,94 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF6CA6F-27A7-496D-AC43-B59BA7833C62}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="12.25" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.4140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.08203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="8.9140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="5" customFormat="1"/>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.5" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="L7" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F238A175-69C8-4527-8C42-E677327AD5E2}">
+          <x14:formula1>
+            <xm:f>Planilha2!$AB$2:$AB$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>A3:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5784BB39-882A-4B77-BB10-D5CA2709706E}">
+          <x14:formula1>
+            <xm:f>Planilha2!$AD$2:$AD$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{81BBD334-7D97-4B2B-ADCD-16787C225511}">
+          <x14:formula1>
+            <xm:f>Planilha2!$AC$2:$AC$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remoção de atividades vindas do space
</commit_message>
<xml_diff>
--- a/Config_Grade.xlsx
+++ b/Config_Grade.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafaeldbo1\Downloads\code\grade_graduacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\Workspaces\Secretaria-Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B10FF1-140A-4F8B-8CC3-3ADA7AA58271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410EBEBA-7928-4574-ABC1-E1A2FFFC14F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Adição Horários Manuais'!$A$2:$J$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Dados Configuráveis'!$A$2:$C$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Remoção Horários Space'!$A$2:$G$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="110">
   <si>
     <t>Tipo</t>
   </si>
@@ -335,23 +336,55 @@
     <t>Turma</t>
   </si>
   <si>
-    <t>Código da Disciplina</t>
-  </si>
-  <si>
     <t>Nome Disciplina</t>
   </si>
   <si>
     <t>Tipo Atividade</t>
   </si>
   <si>
-    <t>GRENGCOM_201561_0023</t>
+    <t>Nome da Disciplina</t>
+  </si>
+  <si>
+    <t>ACIONAMENTOS ELÉTRICOS</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Letra da Turma </t>
+  </si>
+  <si>
+    <t>Período</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuso seguindo  a nova nomenclatura </t>
+  </si>
+  <si>
+    <t>Explicação das Abas</t>
+  </si>
+  <si>
+    <t>Adição Horários Manuais</t>
+  </si>
+  <si>
+    <t>Remoção Horários Space</t>
+  </si>
+  <si>
+    <t>Nessa aba você pode inserir algumas informações para auxiliar a automação a criar a grade corretamente. 
+Essas informações podem ser nome de monitores, disciplinas que possuem um intervalo entre as aulas, monitorias ninjas que devam aparecer na grade, etc.</t>
+  </si>
+  <si>
+    <t>Essa aba permite remover atividades vindas do banco de dados do Space. Para isso preencha as colunas com as informações das aulas que você deseja remover. As colunas: "Curso", "Série", "Turma" e "Nome da Disciplina" são obrigatórias, mas caso você precise remover atividades específicas você também pode preencher as colunas "Tipo de Atividade" e/ou "Dia da Semana".</t>
+  </si>
+  <si>
+    <t>Nessa aba é possível adicionar atividades manualmente na grade. Utilize isso para colocar atividades que por um acaso não estão aparecendo ou para dar mais liberdade durante a construção da grade.
+Atividades adicionadas nesta aba não possuem nenhuma prioridade sobre as atividades vindas do banco de dados do Space. Por isso, caso haja um conflito e essa atividade adicionada manualmente não apareça, será necessário remover a atividade conflitante utilizando a aba "Remoção Horários Space".</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,8 +442,44 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +489,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,9 +534,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -474,14 +546,57 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -822,146 +937,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ACDB79-7005-4B8E-AC77-4D96767B7990}">
-  <dimension ref="AA1:AD11"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AC15" sqref="AC15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="27" max="27" width="37.9140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.75" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.9140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.9140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" style="26" customWidth="1"/>
+    <col min="3" max="26" width="8.88671875" style="20"/>
+    <col min="27" max="27" width="37.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.77734375" style="22" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="27:30">
-      <c r="AA1" s="8" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AA1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="27:30">
-      <c r="AA2" s="3" t="s">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="27:30">
-      <c r="AA3" s="3" t="s">
+    <row r="3" spans="1:30" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="AC3" s="4" t="s">
+      <c r="AC3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AD3" s="22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="27:30">
-      <c r="AA4" s="3" t="s">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B4" s="28"/>
+      <c r="AA4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AB4" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AC4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AD4" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="27:30">
-      <c r="AA5" s="3" t="s">
+    <row r="5" spans="1:30" ht="144" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA5" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AB5" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AC5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AD5" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="27:30">
-      <c r="AA6" s="4" t="s">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="AA6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AB6" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="AC6" s="4" t="s">
+      <c r="AC6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AD6" s="4" t="s">
+      <c r="AD6" s="22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="27:30">
-      <c r="AA7" s="4" t="s">
+    <row r="7" spans="1:30" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA7" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AB7" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="AC7" s="4" t="s">
+      <c r="AC7" s="22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="27:30">
-      <c r="AA8" s="4" t="s">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="AA8" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="AB8" s="4" t="s">
+      <c r="AB8" s="22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="27:30">
-      <c r="AA9" s="4" t="s">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" s="25"/>
+      <c r="AA9" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" s="4" t="s">
+      <c r="AB9" s="22" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="27:30">
-      <c r="AA10" s="4" t="s">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="AA10" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="AB10" s="4" t="s">
+      <c r="AB10" s="22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="27:30">
-      <c r="AB11" s="4" t="s">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" s="25"/>
+      <c r="AB11" s="22" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -969,324 +1116,321 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.9140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.58203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.75" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.9140625" style="3"/>
+    <col min="1" max="1" width="37.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="28">
+    <row r="24" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="28">
-      <c r="A36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="10" t="s">
+    <row r="36" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:C2" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}"/>
@@ -1312,26 +1456,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8DDCAC-6EF5-4B90-A60D-BF7A19FDB345}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.4140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.4140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="18.25" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" style="4" customWidth="1"/>
     <col min="8" max="8" width="16" style="4" customWidth="1"/>
     <col min="9" max="9" width="37.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.6640625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="8.9140625" style="4"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" ht="28">
+    <row r="1" spans="1:15" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="D1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1345,7 +1498,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1356,10 +1509,10 @@
         <v>95</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>98</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>37</v>
@@ -1377,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="42">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
@@ -1402,14 +1555,14 @@
       <c r="H3" s="7">
         <v>0.5</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>45</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="42">
+    <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>89</v>
       </c>
@@ -1438,7 +1591,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="42">
+    <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>88</v>
       </c>
@@ -1463,14 +1616,14 @@
       <c r="H5" s="7">
         <v>0.5</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>45</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="42">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>87</v>
       </c>
@@ -1495,14 +1648,14 @@
       <c r="H6" s="7">
         <v>0.5</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>45</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="28">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>85</v>
       </c>
@@ -1524,15 +1677,15 @@
       <c r="G7" s="7">
         <v>0.3125</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="7">
         <v>0.75</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="1:15" ht="28">
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>89</v>
       </c>
@@ -1561,7 +1714,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="28">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>88</v>
       </c>
@@ -1590,7 +1743,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="28">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -1619,7 +1772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28">
+    <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>91</v>
       </c>
@@ -1648,7 +1801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28">
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>91</v>
       </c>
@@ -1677,7 +1830,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28">
+    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -1709,7 +1862,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="28">
+    <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>85</v>
       </c>
@@ -1741,7 +1894,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="28">
+    <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>85</v>
       </c>
@@ -1773,7 +1926,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="28">
+    <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +1958,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28">
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>85</v>
       </c>
@@ -1837,7 +1990,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28">
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>85</v>
       </c>
@@ -1869,7 +2022,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="28">
+    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>85</v>
       </c>
@@ -1901,7 +2054,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="28">
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
@@ -1967,26 +2120,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF6CA6F-27A7-496D-AC43-B59BA7833C62}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.4140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="5" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" style="5" customWidth="1"/>
-    <col min="8" max="16384" width="8.9140625" style="4"/>
+    <col min="8" max="8" width="35.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1"/>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.5" customHeight="1">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="18.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1997,10 +2165,10 @@
         <v>95</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>37</v>
@@ -2008,8 +2176,9 @@
       <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
@@ -2020,14 +2189,92 @@
         <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="18"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="L7" s="9"/>
+      <c r="E4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G8" s="14"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="14"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2" xr:uid="{3BF6CA6F-27A7-496D-AC43-B59BA7833C62}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -2035,19 +2282,19 @@
           <x14:formula1>
             <xm:f>Planilha2!$AB$2:$AB$11</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A1048576</xm:sqref>
+          <xm:sqref>A3:A10000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5784BB39-882A-4B77-BB10-D5CA2709706E}">
           <x14:formula1>
             <xm:f>Planilha2!$AD$2:$AD$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F1048576</xm:sqref>
+          <xm:sqref>F3:F10000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{81BBD334-7D97-4B2B-ADCD-16787C225511}">
           <x14:formula1>
             <xm:f>Planilha2!$AC$2:$AC$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
+          <xm:sqref>E3:E10000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Mudando para acesso ao lake
</commit_message>
<xml_diff>
--- a/Config_Grade.xlsx
+++ b/Config_Grade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\Workspaces\Secretaria-Workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410EBEBA-7928-4574-ABC1-E1A2FFFC14F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D352B304-6AD2-486C-B0BE-AEFEB83B5802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F1820AC4-512B-4897-8625-578DC14BB6C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="109">
   <si>
     <t>Tipo</t>
   </si>
@@ -297,9 +297,6 @@
     <t>Nova Grade</t>
   </si>
   <si>
-    <t>NÃO</t>
-  </si>
-  <si>
     <t>MICROECONOMIA I</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
   </si>
   <si>
     <t>ACIONAMENTOS ELÉTRICOS</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t xml:space="preserve">Letra da Turma </t>
@@ -378,6 +372,9 @@
   <si>
     <t>Nessa aba é possível adicionar atividades manualmente na grade. Utilize isso para colocar atividades que por um acaso não estão aparecendo ou para dar mais liberdade durante a construção da grade.
 Atividades adicionadas nesta aba não possuem nenhuma prioridade sobre as atividades vindas do banco de dados do Space. Por isso, caso haja um conflito e essa atividade adicionada manualmente não apareça, será necessário remover a atividade conflitante utilizando a aba "Remoção Horários Space".</t>
+  </si>
+  <si>
+    <t>SIM</t>
   </si>
 </sst>
 </file>
@@ -583,16 +580,16 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -939,7 +936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ACDB79-7005-4B8E-AC77-4D96767B7990}">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -971,13 +968,13 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AA2" s="21" t="s">
         <v>61</v>
       </c>
       <c r="AB2" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AC2" s="22" t="s">
         <v>27</v>
@@ -991,13 +988,13 @@
         <v>23</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AA3" s="21" t="s">
         <v>16</v>
       </c>
       <c r="AB3" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC3" s="22" t="s">
         <v>26</v>
@@ -1012,7 +1009,7 @@
         <v>17</v>
       </c>
       <c r="AB4" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC4" s="22" t="s">
         <v>29</v>
@@ -1023,16 +1020,16 @@
     </row>
     <row r="5" spans="1:30" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AA5" s="21" t="s">
         <v>48</v>
       </c>
       <c r="AB5" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AC5" s="22" t="s">
         <v>28</v>
@@ -1047,7 +1044,7 @@
         <v>30</v>
       </c>
       <c r="AB6" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AC6" s="22" t="s">
         <v>30</v>
@@ -1058,16 +1055,16 @@
     </row>
     <row r="7" spans="1:30" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>106</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>108</v>
       </c>
       <c r="AA7" s="22" t="s">
         <v>58</v>
       </c>
       <c r="AB7" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC7" s="22" t="s">
         <v>55</v>
@@ -1079,7 +1076,7 @@
         <v>69</v>
       </c>
       <c r="AB8" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
@@ -1088,7 +1085,7 @@
         <v>77</v>
       </c>
       <c r="AB9" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
@@ -1097,13 +1094,13 @@
         <v>82</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="25"/>
       <c r="AB11" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1114,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1384,7 +1381,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>69</v>
       </c>
@@ -1392,7 +1389,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -1400,7 +1397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1408,29 +1405,35 @@
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="B36" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:C2" xr:uid="{DE5930CE-E02D-42FA-8581-5FB2511141DA}"/>
@@ -1456,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8DDCAC-6EF5-4B90-A60D-BF7A19FDB345}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,13 +1480,13 @@
   <sheetData>
     <row r="1" spans="1:15" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>34</v>
@@ -1506,13 +1509,13 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>97</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>37</v>
@@ -1532,7 +1535,7 @@
     </row>
     <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="4">
         <v>6</v>
@@ -1564,7 +1567,7 @@
     </row>
     <row r="4" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
@@ -1593,7 +1596,7 @@
     </row>
     <row r="5" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4">
         <v>8</v>
@@ -1625,7 +1628,7 @@
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="4">
         <v>8</v>
@@ -1657,7 +1660,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
@@ -1687,7 +1690,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="4">
         <v>8</v>
@@ -1716,7 +1719,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
@@ -1745,7 +1748,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
@@ -1774,7 +1777,7 @@
     </row>
     <row r="11" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="4">
         <v>6</v>
@@ -1803,7 +1806,7 @@
     </row>
     <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="4">
         <v>6</v>
@@ -1832,7 +1835,7 @@
     </row>
     <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
@@ -1864,7 +1867,7 @@
     </row>
     <row r="14" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
@@ -1896,7 +1899,7 @@
     </row>
     <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
@@ -1928,7 +1931,7 @@
     </row>
     <row r="16" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -1960,7 +1963,7 @@
     </row>
     <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -1992,7 +1995,7 @@
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -2024,7 +2027,7 @@
     </row>
     <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
@@ -2122,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF6CA6F-27A7-496D-AC43-B59BA7833C62}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2141,13 +2144,13 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>34</v>
@@ -2162,13 +2165,13 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>37</v>
@@ -2180,75 +2183,30 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B3" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>98</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="G5" s="14"/>
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>